<commit_message>
add trial info for 1399 Dx cohort.
</commit_message>
<xml_diff>
--- a/data/tableone_both_cohorts.xlsx
+++ b/data/tableone_both_cohorts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Grouped by cohort</t>
   </si>
@@ -52,6 +52,9 @@
     <t>Treatment Arm, n (%)</t>
   </si>
   <si>
+    <t>Clinical Trial, n (%)</t>
+  </si>
+  <si>
     <t>≥10</t>
   </si>
   <si>
@@ -97,6 +100,36 @@
     <t>Arm B</t>
   </si>
   <si>
+    <t>AAML03P1</t>
+  </si>
+  <si>
+    <t>AAML0531</t>
+  </si>
+  <si>
+    <t>AAML1031</t>
+  </si>
+  <si>
+    <t>Beat AML Consortium</t>
+  </si>
+  <si>
+    <t>CCG2961</t>
+  </si>
+  <si>
+    <t>CETLAM SMD-09 (MDS-tAML)</t>
+  </si>
+  <si>
+    <t>Japanese AML05</t>
+  </si>
+  <si>
+    <t>TCGA AML</t>
+  </si>
+  <si>
+    <t>AML02</t>
+  </si>
+  <si>
+    <t>AML08</t>
+  </si>
+  <si>
     <t>516 (47.6)</t>
   </si>
   <si>
@@ -142,6 +175,30 @@
     <t>313 (56.4)</t>
   </si>
   <si>
+    <t>60 (4.3)</t>
+  </si>
+  <si>
+    <t>496 (35.5)</t>
+  </si>
+  <si>
+    <t>487 (34.8)</t>
+  </si>
+  <si>
+    <t>182 (13.0)</t>
+  </si>
+  <si>
+    <t>31 (2.2)</t>
+  </si>
+  <si>
+    <t>83 (5.9)</t>
+  </si>
+  <si>
+    <t>9 (0.6)</t>
+  </si>
+  <si>
+    <t>51 (3.6)</t>
+  </si>
+  <si>
     <t>452 (48.9)</t>
   </si>
   <si>
@@ -187,6 +244,15 @@
     <t>274 (52.1)</t>
   </si>
   <si>
+    <t>36 (3.9)</t>
+  </si>
+  <si>
+    <t>491 (53.1)</t>
+  </si>
+  <si>
+    <t>397 (43.0)</t>
+  </si>
+  <si>
     <t>95 (47.7)</t>
   </si>
   <si>
@@ -227,6 +293,12 @@
   </si>
   <si>
     <t>92 (46.2)</t>
+  </si>
+  <si>
+    <t>159 (79.1)</t>
+  </si>
+  <si>
+    <t>42 (20.9)</t>
   </si>
 </sst>
 </file>
@@ -584,7 +656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -630,31 +702,31 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -662,31 +734,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -694,31 +766,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -726,31 +798,31 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -758,46 +830,46 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -805,31 +877,31 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -837,35 +909,136 @@
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
         <v>56</v>
       </c>
-      <c r="E19" t="s">
-        <v>70</v>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
@@ -874,6 +1047,7 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>